<commit_message>
Fuck, csv reader doesn't work
</commit_message>
<xml_diff>
--- a/Assets/2-Scripts/All choices.xlsx
+++ b/Assets/2-Scripts/All choices.xlsx
@@ -691,9 +691,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -728,6 +725,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,7 +853,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -981,11 +980,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="157365760"/>
-        <c:axId val="157367296"/>
+        <c:axId val="201516928"/>
+        <c:axId val="201518464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157365760"/>
+        <c:axId val="201516928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,7 +1022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157367296"/>
+        <c:crossAx val="201518464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1031,7 +1030,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157367296"/>
+        <c:axId val="201518464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,7 +1075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157365760"/>
+        <c:crossAx val="201516928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1153,7 +1152,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1249,11 +1247,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="157396352"/>
-        <c:axId val="157406336"/>
+        <c:axId val="202076160"/>
+        <c:axId val="202077696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157396352"/>
+        <c:axId val="202076160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157406336"/>
+        <c:crossAx val="202077696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1299,7 +1297,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157406336"/>
+        <c:axId val="202077696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1342,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157396352"/>
+        <c:crossAx val="202076160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1421,7 +1419,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1517,11 +1514,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190924288"/>
-        <c:axId val="190925824"/>
+        <c:axId val="202446720"/>
+        <c:axId val="202448256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190924288"/>
+        <c:axId val="202446720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190925824"/>
+        <c:crossAx val="202448256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1564,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190925824"/>
+        <c:axId val="202448256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,7 +1609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190924288"/>
+        <c:crossAx val="202446720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1689,7 +1686,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1785,11 +1781,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190934400"/>
-        <c:axId val="190948480"/>
+        <c:axId val="202485760"/>
+        <c:axId val="202487296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190934400"/>
+        <c:axId val="202485760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +1823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190948480"/>
+        <c:crossAx val="202487296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1835,7 +1831,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190948480"/>
+        <c:axId val="202487296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +1876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190934400"/>
+        <c:crossAx val="202485760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2343,47 +2339,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -2411,7 +2407,7 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J4">
@@ -2444,7 +2440,7 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J5">
@@ -2504,9 +2500,9 @@
       <c r="G7">
         <v>2</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -2534,11 +2530,11 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -2566,7 +2562,7 @@
       <c r="G9">
         <v>2</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J9">
@@ -2599,7 +2595,7 @@
       <c r="G10">
         <v>2</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J10">
@@ -2634,19 +2630,19 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J14">
@@ -2654,7 +2650,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J15">
@@ -2662,19 +2658,19 @@
       </c>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J19">
@@ -2682,7 +2678,7 @@
       </c>
     </row>
     <row r="20" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J20">
@@ -2690,18 +2686,18 @@
       </c>
     </row>
     <row r="22" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="23" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J24">
@@ -2748,67 +2744,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2825,10 +2821,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2843,7 +2839,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
     </row>
@@ -2860,7 +2856,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
     </row>
@@ -2877,29 +2873,29 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
     </row>
@@ -2916,7 +2912,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
     </row>
@@ -2933,7 +2929,7 @@
       <c r="E9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
     </row>
@@ -2950,7 +2946,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
     </row>
@@ -2967,23 +2963,23 @@
       <c r="E11">
         <v>1.5</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
     </row>
@@ -2994,7 +2990,7 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -3005,7 +3001,7 @@
       <c r="B15">
         <v>0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -3016,7 +3012,7 @@
       <c r="B16">
         <v>0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -3027,27 +3023,27 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -3088,67 +3084,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3165,10 +3161,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3183,7 +3179,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
     </row>
@@ -3200,7 +3196,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
     </row>
@@ -3217,29 +3213,29 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
     </row>
@@ -3256,7 +3252,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
     </row>
@@ -3273,7 +3269,7 @@
       <c r="E9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
     </row>
@@ -3290,7 +3286,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
     </row>
@@ -3307,23 +3303,23 @@
       <c r="E11">
         <v>1.5</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
     </row>
@@ -3334,7 +3330,7 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -3345,7 +3341,7 @@
       <c r="B15">
         <v>0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -3356,7 +3352,7 @@
       <c r="B16">
         <v>0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -3367,27 +3363,27 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -3430,67 +3426,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3507,10 +3503,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3525,7 +3521,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
     </row>
@@ -3542,7 +3538,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
     </row>
@@ -3559,29 +3555,29 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
     </row>
@@ -3598,7 +3594,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
     </row>
@@ -3615,7 +3611,7 @@
       <c r="E9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
     </row>
@@ -3632,7 +3628,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
     </row>
@@ -3649,23 +3645,23 @@
       <c r="E11">
         <v>1.5</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
     </row>
@@ -3676,7 +3672,7 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -3687,7 +3683,7 @@
       <c r="B15">
         <v>0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -3698,7 +3694,7 @@
       <c r="B16">
         <v>0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -3709,27 +3705,27 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -3772,67 +3768,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3849,10 +3845,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3867,7 +3863,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
     </row>
@@ -3884,7 +3880,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
     </row>
@@ -3901,29 +3897,29 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
     </row>
@@ -3940,7 +3936,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
     </row>
@@ -3957,7 +3953,7 @@
       <c r="E9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
     </row>
@@ -3974,7 +3970,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
     </row>
@@ -3991,23 +3987,23 @@
       <c r="E11">
         <v>1.5</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
     </row>
@@ -4018,7 +4014,7 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -4029,7 +4025,7 @@
       <c r="B15">
         <v>0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -4040,7 +4036,7 @@
       <c r="B16">
         <v>0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -4051,27 +4047,27 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -4106,64 +4102,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4180,7 +4176,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -4212,7 +4208,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" t="s">
@@ -4244,7 +4240,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -4276,7 +4272,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
       <c r="H5" t="s">
@@ -4296,24 +4292,24 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
     </row>
@@ -4330,7 +4326,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
     </row>
@@ -4347,7 +4343,7 @@
       <c r="E9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
     </row>
@@ -4364,7 +4360,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
     </row>
@@ -4381,23 +4377,23 @@
       <c r="E11">
         <v>1.5</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
     </row>
@@ -4408,7 +4404,7 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -4419,7 +4415,7 @@
       <c r="B15">
         <v>0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -4430,7 +4426,7 @@
       <c r="B16">
         <v>0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -4441,27 +4437,27 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -4490,57 +4486,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2">
@@ -4565,7 +4561,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3">
@@ -4590,7 +4586,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4">
@@ -4615,7 +4611,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5">
@@ -4640,7 +4636,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6">
@@ -4665,7 +4661,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -4690,7 +4686,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8">
@@ -4715,7 +4711,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9">
@@ -4740,7 +4736,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10">
@@ -4765,7 +4761,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11">
@@ -4790,7 +4786,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12">
@@ -4815,7 +4811,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13">
@@ -4840,42 +4836,42 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -4914,67 +4910,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4991,7 +4987,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -5029,7 +5025,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" t="s">
@@ -5064,7 +5060,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -5099,7 +5095,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
       <c r="H5" t="s">
@@ -5134,7 +5130,7 @@
       <c r="E6">
         <v>-0.3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
       <c r="H6" t="s">
@@ -5169,7 +5165,7 @@
       <c r="E7">
         <v>-0.6</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
@@ -5204,7 +5200,7 @@
       <c r="E8">
         <v>-0.9</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
       <c r="H8" t="s">
@@ -5227,7 +5223,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
       <c r="H9" t="s">
@@ -5253,19 +5249,19 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="7"/>
       <c r="H10" t="s">
         <v>37</v>
       </c>
@@ -5301,7 +5297,7 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>9</v>
       </c>
       <c r="H11" t="s">
@@ -5339,7 +5335,7 @@
       <c r="E12">
         <v>0.5</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>10</v>
       </c>
       <c r="H12" t="s">
@@ -5374,7 +5370,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>11</v>
       </c>
       <c r="H13" t="s">
@@ -5409,7 +5405,7 @@
       <c r="E14">
         <v>1.5</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>12</v>
       </c>
       <c r="H14" t="s">
@@ -5444,7 +5440,7 @@
       <c r="E15">
         <v>-0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>13</v>
       </c>
       <c r="H15" t="s">
@@ -5479,7 +5475,7 @@
       <c r="E16">
         <v>-0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>14</v>
       </c>
       <c r="H16" t="s">
@@ -5514,7 +5510,7 @@
       <c r="E17">
         <v>-0.9</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>15</v>
       </c>
       <c r="H17" t="s">
@@ -5537,7 +5533,7 @@
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>16</v>
       </c>
       <c r="H18" t="s">
@@ -5560,13 +5556,13 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>17</v>
       </c>
       <c r="H19" t="s">
@@ -5598,7 +5594,7 @@
       <c r="B20">
         <v>0</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>18</v>
       </c>
       <c r="H20" t="s">
@@ -5633,7 +5629,7 @@
       <c r="B21">
         <v>0.3</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>19</v>
       </c>
       <c r="H21" t="s">
@@ -5668,7 +5664,7 @@
       <c r="B22">
         <v>0.6</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>20</v>
       </c>
       <c r="H22" t="s">
@@ -5772,60 +5768,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2">
@@ -5894,7 +5890,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3">
@@ -5963,7 +5959,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4">
@@ -6032,7 +6028,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5">
@@ -6101,7 +6097,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6">
@@ -6170,7 +6166,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -6239,7 +6235,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8">
@@ -6308,7 +6304,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9">
@@ -6377,7 +6373,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10">
@@ -6446,7 +6442,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11">
@@ -6515,7 +6511,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12">
@@ -6584,7 +6580,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13">
@@ -6653,7 +6649,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14">
@@ -6722,7 +6718,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15">
@@ -6791,7 +6787,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16">
@@ -6860,7 +6856,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17">
@@ -6929,7 +6925,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18">
@@ -6998,7 +6994,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19">
@@ -7067,7 +7063,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20">
@@ -7136,7 +7132,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21">
@@ -7365,67 +7361,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -7442,7 +7438,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -7480,7 +7476,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" t="s">
@@ -7518,7 +7514,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -7556,7 +7552,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
       <c r="H5" t="s">
@@ -7594,7 +7590,7 @@
       <c r="E6">
         <v>-0.3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
       <c r="H6" t="s">
@@ -7632,7 +7628,7 @@
       <c r="E7">
         <v>-0.6</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
@@ -7653,7 +7649,7 @@
       <c r="M7" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="15" t="s">
+      <c r="W7" s="14" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7670,7 +7666,7 @@
       <c r="E8">
         <v>-0.9</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
       <c r="H8" t="s">
@@ -7696,7 +7692,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
       <c r="H9" t="s">
@@ -7722,19 +7718,19 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
       <c r="H10" t="s">
@@ -7775,7 +7771,7 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
       <c r="H11" t="s">
@@ -7813,7 +7809,7 @@
       <c r="E12">
         <v>0.5</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
       <c r="H12" t="s">
@@ -7854,7 +7850,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
       <c r="H13" t="s">
@@ -7892,7 +7888,7 @@
       <c r="E14">
         <v>1.5</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -7909,7 +7905,7 @@
       <c r="E15">
         <v>-0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -7926,7 +7922,7 @@
       <c r="E16">
         <v>-0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -7943,23 +7939,23 @@
       <c r="E17">
         <v>-0.9</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
     </row>
@@ -7970,7 +7966,7 @@
       <c r="B20">
         <v>0</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
     </row>
@@ -7981,7 +7977,7 @@
       <c r="B21">
         <v>0.3</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
     </row>
@@ -8050,60 +8046,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2">
@@ -8172,7 +8168,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3">
@@ -8241,7 +8237,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4">
@@ -8310,7 +8306,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5">
@@ -8379,7 +8375,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6">
@@ -8448,7 +8444,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -8517,7 +8513,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8">
@@ -8586,7 +8582,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9">
@@ -8655,7 +8651,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10">
@@ -8724,7 +8720,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11">
@@ -8793,7 +8789,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12">
@@ -8862,7 +8858,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13">
@@ -8967,67 +8963,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -9044,7 +9040,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -9065,7 +9061,7 @@
       <c r="M2" t="s">
         <v>84</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>85</v>
       </c>
       <c r="O2" t="s">
@@ -9091,7 +9087,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" t="s">
@@ -9135,7 +9131,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -9176,7 +9172,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
       <c r="H5" t="s">
@@ -9223,7 +9219,7 @@
       <c r="E6">
         <v>-0.3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
       <c r="H6" t="s">
@@ -9267,7 +9263,7 @@
       <c r="E7">
         <v>-0.6</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
@@ -9314,7 +9310,7 @@
       <c r="E8">
         <v>-0.9</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
       <c r="H8" t="s">
@@ -9346,7 +9342,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
       <c r="H9" t="s">
@@ -9378,19 +9374,19 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
       <c r="H10" t="s">
@@ -9431,7 +9427,7 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
       <c r="H11" t="s">
@@ -9478,7 +9474,7 @@
       <c r="E12">
         <v>0.5</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
       <c r="H12" t="s">
@@ -9522,7 +9518,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
       <c r="H13" t="s">
@@ -9569,7 +9565,7 @@
       <c r="E14">
         <v>1.5</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
       <c r="H14" t="s">
@@ -9619,7 +9615,7 @@
       <c r="E15">
         <v>-0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
       <c r="H15" t="s">
@@ -9660,7 +9656,7 @@
       <c r="E16">
         <v>-0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
       <c r="H16" t="s">
@@ -9704,7 +9700,7 @@
       <c r="E17">
         <v>-0.9</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
       <c r="H17" t="s">
@@ -9736,7 +9732,7 @@
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
       <c r="H18" t="s">
@@ -9765,13 +9761,13 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
       <c r="H19" t="s">
@@ -9806,7 +9802,7 @@
       <c r="B20">
         <v>0</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
       <c r="H20" t="s">
@@ -9844,7 +9840,7 @@
       <c r="B21">
         <v>0.3</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
       <c r="H21" t="s">
@@ -10254,60 +10250,60 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2">
@@ -10376,7 +10372,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3">
@@ -10445,7 +10441,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4">
@@ -10514,7 +10510,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5">
@@ -10583,7 +10579,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6">
@@ -10652,7 +10648,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -10721,7 +10717,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8">
@@ -10790,7 +10786,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9">
@@ -10859,7 +10855,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10">
@@ -10928,7 +10924,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11">
@@ -10997,7 +10993,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12">
@@ -11066,7 +11062,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13">
@@ -11172,67 +11168,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11249,7 +11245,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -11293,7 +11289,7 @@
       <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" t="s">
@@ -11334,7 +11330,7 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -11378,7 +11374,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
       <c r="H5" t="s">
@@ -11425,7 +11421,7 @@
       <c r="E6">
         <v>-0.3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
       <c r="H6" t="s">
@@ -11472,7 +11468,7 @@
       <c r="E7">
         <v>-0.6</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
@@ -11519,7 +11515,7 @@
       <c r="E8">
         <v>-0.9</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
       <c r="H8" t="s">
@@ -11551,7 +11547,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
       <c r="H9" t="s">
@@ -11586,19 +11582,19 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9</v>
       </c>
       <c r="H10" t="s">
@@ -11642,7 +11638,7 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>10</v>
       </c>
       <c r="H11" t="s">
@@ -11686,7 +11682,7 @@
       <c r="E12">
         <v>0.5</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11</v>
       </c>
       <c r="H12" t="s">
@@ -11730,7 +11726,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>12</v>
       </c>
       <c r="H13" t="s">
@@ -11777,7 +11773,7 @@
       <c r="E14">
         <v>1.5</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>13</v>
       </c>
       <c r="H14" t="s">
@@ -11815,7 +11811,7 @@
       <c r="E15">
         <v>-0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>14</v>
       </c>
       <c r="H15" t="s">
@@ -11850,7 +11846,7 @@
       <c r="E16">
         <v>-0.6</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>15</v>
       </c>
       <c r="H16" t="s">
@@ -11885,7 +11881,7 @@
       <c r="E17">
         <v>-0.9</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>16</v>
       </c>
       <c r="H17" t="s">
@@ -11908,7 +11904,7 @@
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>17</v>
       </c>
       <c r="H18" t="s">
@@ -11931,13 +11927,13 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>18</v>
       </c>
       <c r="H19" t="s">
@@ -11975,7 +11971,7 @@
       <c r="B20">
         <v>0</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>19</v>
       </c>
       <c r="H20" t="s">
@@ -12016,7 +12012,7 @@
       <c r="B21">
         <v>0.3</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>20</v>
       </c>
       <c r="H21" t="s">
@@ -12613,67 +12609,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2">
@@ -12742,7 +12738,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3">
@@ -12811,7 +12807,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4">
@@ -12880,7 +12876,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5">
@@ -12949,7 +12945,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6">
@@ -13018,7 +13014,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -13087,7 +13083,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8">
@@ -13156,7 +13152,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9">
@@ -13225,7 +13221,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10">
@@ -13294,7 +13290,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11">
@@ -13363,7 +13359,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12">
@@ -13432,7 +13428,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13">
@@ -13501,6 +13497,9 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
       <c r="B14">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H14,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -13567,6 +13566,9 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
       <c r="B15">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H15,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -13633,6 +13635,9 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
       <c r="B16">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H16,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -13698,7 +13703,10 @@
         <v>Go to the zoo with parents</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
       <c r="B17">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H17,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>27</v>
@@ -13764,7 +13772,10 @@
         <v>Go to the beach with parents</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
       <c r="B18">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H18,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>27</v>
@@ -13830,7 +13841,10 @@
         <v>Go to the park with parents</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
       <c r="B19">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H19,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>27</v>
@@ -13896,7 +13910,10 @@
         <v>Play outside with friends</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
       <c r="B20">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H20,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -13962,7 +13979,10 @@
         <v>Watch movies with friends</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
       <c r="B21">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H21,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -14028,7 +14048,10 @@
         <v>Read at home</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
       <c r="B22">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H22,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -14094,7 +14117,10 @@
         <v>Read storybooks</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
       <c r="B23">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H23,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -14160,7 +14186,10 @@
         <v>Study school material</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
       <c r="B24">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H24,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -14226,7 +14255,10 @@
         <v>Read the biography of Steve Jobs</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
       <c r="B25">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H25,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -14292,7 +14324,10 @@
         <v>Ask parents to buy my favorite toy gun!</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
       <c r="B26">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H26,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -14358,7 +14393,10 @@
         <v>Buy with my own money</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
       <c r="B27">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H27,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -14424,7 +14462,10 @@
         <v>Window shopping</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
       <c r="B28">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H28,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -14490,7 +14531,10 @@
         <v>Attend tuition class</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
       <c r="B29">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H29,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -14556,7 +14600,10 @@
         <v>Pretend to be ill</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
       <c r="B30">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H30,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -14622,7 +14669,10 @@
         <v>Screw the tuition class and don’t go anymore</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
       <c r="B31">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H31,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>14</v>
@@ -14688,7 +14738,10 @@
         <v>Draw</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
       <c r="B32">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H32,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>14</v>
@@ -14754,7 +14807,10 @@
         <v>Play with toys</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
       <c r="B33">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H33,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>14</v>
@@ -14820,7 +14876,10 @@
         <v xml:space="preserve">Sleep </v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
       <c r="B34">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H34,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>14</v>
@@ -14886,7 +14945,10 @@
         <v>Fold paper plane</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
       <c r="B35">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H35,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>20</v>
@@ -14952,7 +15014,10 @@
         <v>Watch TV</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
       <c r="B36">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H36,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>27</v>
@@ -15018,7 +15083,10 @@
         <v>Do homework with the best effort</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
       <c r="B37">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H37,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>14</v>
@@ -15084,7 +15152,10 @@
         <v>Cincai do homework</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
       <c r="B38">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H38,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -15150,7 +15221,10 @@
         <v>Screw the homework, I’ll copy my friends’ tomorrow</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
       <c r="B39">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H39,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -15216,7 +15290,10 @@
         <v>Seeing neighbor has a new toy, ask parents to buy</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
       <c r="B40">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H40,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -15282,7 +15359,10 @@
         <v>Seeing neighbor has a new toy, buy with my own money</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
       <c r="B41">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H41,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>0</v>
@@ -15348,7 +15428,10 @@
         <v>Seeing neighbor has a new toy, I can only dream about it</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>41</v>
+      </c>
       <c r="B42">
         <f>ROUND(VLOOKUP('4-PreteenChoice'!H42,'4-PreteenChoice'!$A$2:$B$8,2,FALSE) * StandardChoice!C$7,0)</f>
         <v>14</v>

</xml_diff>